<commit_message>
updated controller and demo template files
</commit_message>
<xml_diff>
--- a/Template/Google.xlsx
+++ b/Template/Google.xlsx
@@ -12,7 +12,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+  <si>
+    <t>ScriptType</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
   <si>
     <t>TCID</t>
   </si>
@@ -23,6 +29,9 @@
     <t>TAG</t>
   </si>
   <si>
+    <t>DependsOn</t>
+  </si>
+  <si>
     <t>Component</t>
   </si>
   <si>
@@ -30,6 +39,15 @@
   </si>
   <si>
     <t>URL</t>
+  </si>
+  <si>
+    <t>alert</t>
+  </si>
+  <si>
+    <t>confirm</t>
+  </si>
+  <si>
+    <t>prompt</t>
   </si>
 </sst>
 </file>
@@ -74,40 +92,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="C1" t="s">
-        <v>3</v>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2">
-      <c r="C2" t="s">
-        <v>4</v>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>